<commit_message>
Added percent compare function
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/SignalIndicator_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/SignalIndicator_JS.xlsx
@@ -387,28 +387,6 @@
 TakeScreenshot(VT200-0851);</t>
   </si>
   <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Signal JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0862
-};
-validate4
-{
-validate_Screenshot=VT200-0861-01
-};
-validate5
-{
-validate_Screenshot=VT200-0861-02
-};</t>
-  </si>
-  <si>
     <t xml:space="preserve">validate1
 {
 validate_PageTitle=Compliance JS specs
@@ -571,6 +549,28 @@
 checkCallbackValues(ipwlandisable_xpath);
 wifi_Mode(ON);
 press_Key(Home);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Signal JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0861
+};
+validate4
+{
+validate_Screenshot=VT200-0861-01
+};
+validate5
+{
+validate_Screenshot=VT200-0861-02
+};</t>
   </si>
 </sst>
 </file>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1065,10 +1065,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1308,10 +1308,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1335,10 +1335,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1362,10 +1362,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>

</xml_diff>

<commit_message>
Fixed Signal issue in selendroid
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/SignalIndicator_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/SignalIndicator_JS.xlsx
@@ -372,21 +372,6 @@
 };</t>
   </si>
   <si>
-    <t>wait(3);
-validate1;
-link_Click(signal_test_link);
-validate2;
-SelectTestToRun(VT200_0851_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-TakeScreenshot(VT200-0851);
-validate4;
-wait(2);
-TakeScreenshot(VT200-0851);</t>
-  </si>
-  <si>
     <t xml:space="preserve">validate1
 {
 validate_PageTitle=Compliance JS specs
@@ -571,6 +556,24 @@
 {
 validate_Screenshot=VT200-0861-02
 };</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(VT200_0851_home_xpath);
+SwitchApp(WEBVIEW);
+link_Click(signal_test_link);
+validate2;
+SelectTestToRun(VT200_0851_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+TakeScreenshot(VT200-0851);
+validate4;
+wait(2);
+TakeScreenshot(VT200-0851);</t>
   </si>
 </sst>
 </file>
@@ -970,7 +973,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1016,7 +1019,7 @@
       </c>
       <c r="K1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="180.75" thickBot="1">
+    <row r="2" spans="1:11" ht="192" thickBot="1">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>42</v>
@@ -1065,10 +1068,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1308,10 +1311,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1335,10 +1338,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1362,10 +1365,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>

</xml_diff>

<commit_message>
Modified appgallery_test to Rhomobile and added EB support
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/SignalIndicator_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/SignalIndicator_JS.xlsx
@@ -221,24 +221,6 @@
 };
 validate3
 {
-validate_Text_Exists=VT200-0855
-};
-validate4
-{
-validate_Screenshot=VT200_0855
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Signal JS Test
-};
-validate3
-{
 validate_Text_Exists=VT200-0859
 };
 validate4
@@ -574,6 +556,24 @@
 validate4;
 wait(2);
 TakeScreenshot(VT200-0851);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Signal JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0855
+};
+validate4
+{
+validate_Screenshot=VT200-0855
+};</t>
   </si>
 </sst>
 </file>
@@ -973,7 +973,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1039,10 +1039,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>12</v>
@@ -1068,10 +1068,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1098,7 +1098,7 @@
         <v>26</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1125,7 +1125,7 @@
         <v>27</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1152,7 +1152,7 @@
         <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1179,7 +1179,7 @@
         <v>29</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1206,7 +1206,7 @@
         <v>30</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1233,7 +1233,7 @@
         <v>31</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1260,7 +1260,7 @@
         <v>32</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1287,7 +1287,7 @@
         <v>33</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1311,10 +1311,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1338,10 +1338,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1365,10 +1365,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>

</xml_diff>

<commit_message>
Modified signal callback function
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/SignalIndicator_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/SignalIndicator_JS.xlsx
@@ -457,6 +457,84 @@
 </t>
   </si>
   <si>
+    <t>wait(3);
+validate1;
+link_Click(signal_test_link);
+validate2;
+SelectTestToRun(VT200_0864_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+wifi_Mode(OFF);
+wait(2);
+press_Key(Home);
+launch_App_Device(com.rhomobile.compliancetest_js/com.rhomobile.rhodes.RhodesActivity);
+wait(2);
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+validate4;
+checkCallbackValues(ipwlandisable_xpath);
+wifi_Mode(ON);
+press_Key(Home);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Signal JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0861
+};
+validate4
+{
+validate_Screenshot=VT200-0861-01
+};
+validate5
+{
+validate_Screenshot=VT200-0861-02
+};</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+SwitchApp(NATIVE_APP);
+ClickNativeIcon(VT200_0851_home_xpath);
+SwitchApp(WEBVIEW);
+link_Click(signal_test_link);
+validate2;
+SelectTestToRun(VT200_0851_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(2);
+TakeScreenshot(VT200-0851);
+validate4;
+wait(2);
+TakeScreenshot(VT200-0851);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Signal JS Test
+};
+validate3
+{
+validate_Text_Exists=VT200-0855
+};
+validate4
+{
+validate_Screenshot=VT200-0855
+};</t>
+  </si>
+  <si>
     <t xml:space="preserve">wait(3);
 validate1;
 link_Click(signal_test_link);
@@ -477,7 +555,7 @@
 checkCallbackValues(essid_xpath);
 checkCallbackValues(ipaddress_xpath);
 checkCallbackValues(signalStrength_xpath);
-signalCallbackcount(results_id);
+signalCallbackcount(results_id,com.rhomobile.compliancetest_js/com.rhomobile.rhodes.RhodesActivity);
 </t>
   </si>
   <si>
@@ -495,85 +573,7 @@
 launch_App_Device(com.rhomobile.compliancetest_js/com.rhomobile.rhodes.RhodesActivity);
 validate4;
 wait(15);
-checkstopwlanStatus(results_id);</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(signal_test_link);
-validate2;
-SelectTestToRun(VT200_0864_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-wifi_Mode(OFF);
-wait(2);
-press_Key(Home);
-launch_App_Device(com.rhomobile.compliancetest_js/com.rhomobile.rhodes.RhodesActivity);
-wait(2);
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-validate4;
-checkCallbackValues(ipwlandisable_xpath);
-wifi_Mode(ON);
-press_Key(Home);</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Signal JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0861
-};
-validate4
-{
-validate_Screenshot=VT200-0861-01
-};
-validate5
-{
-validate_Screenshot=VT200-0861-02
-};</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-SwitchApp(NATIVE_APP);
-ClickNativeIcon(VT200_0851_home_xpath);
-SwitchApp(WEBVIEW);
-link_Click(signal_test_link);
-validate2;
-SelectTestToRun(VT200_0851_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(2);
-TakeScreenshot(VT200-0851);
-validate4;
-wait(2);
-TakeScreenshot(VT200-0851);</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Signal JS Test
-};
-validate3
-{
-validate_Text_Exists=VT200-0855
-};
-validate4
-{
-validate_Screenshot=VT200-0855
-};</t>
+checkstopwlanStatus(results_id,com.rhomobile.compliancetest_js/com.rhomobile.rhodes.RhodesActivity);</t>
   </si>
 </sst>
 </file>
@@ -972,9 +972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1039,7 +1037,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>41</v>
@@ -1050,7 +1048,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="304.5" thickBot="1">
+    <row r="3" spans="1:11" ht="315.75" thickBot="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1068,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>42</v>
@@ -1152,7 +1150,7 @@
         <v>28</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1314,7 +1312,7 @@
         <v>44</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1338,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>45</v>
@@ -1365,7 +1363,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>43</v>

</xml_diff>